<commit_message>
add Latn to lang attributes
</commit_message>
<xml_diff>
--- a/new_attributions.xlsx
+++ b/new_attributions.xlsx
@@ -946,7 +946,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -1471,12 +1471,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -1541,7 +1541,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -2626,7 +2626,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -2871,7 +2871,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -2906,7 +2906,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -2976,7 +2976,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -3186,7 +3186,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -3256,7 +3256,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -3291,7 +3291,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -3396,7 +3396,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -3606,7 +3606,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -3676,7 +3676,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -3711,7 +3711,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -3816,7 +3816,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -3851,7 +3851,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -3921,7 +3921,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -3956,7 +3956,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -4096,7 +4096,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -4131,7 +4131,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -4236,7 +4236,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -4306,7 +4306,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -4411,7 +4411,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -4446,7 +4446,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -4516,7 +4516,7 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -4551,7 +4551,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -4621,7 +4621,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -4656,7 +4656,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
@@ -4726,7 +4726,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -4761,7 +4761,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
@@ -4831,7 +4831,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -4866,7 +4866,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
@@ -4971,7 +4971,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
@@ -5111,7 +5111,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
@@ -5251,7 +5251,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
@@ -5286,7 +5286,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
@@ -5391,7 +5391,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
@@ -5566,7 +5566,7 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
@@ -5636,7 +5636,7 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
@@ -5671,7 +5671,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
@@ -5741,7 +5741,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
@@ -5811,7 +5811,7 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
@@ -5881,7 +5881,7 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
@@ -5916,7 +5916,7 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
@@ -5951,7 +5951,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -6021,7 +6021,7 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
@@ -6091,7 +6091,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
@@ -6126,7 +6126,7 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
@@ -6196,7 +6196,7 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
@@ -6231,7 +6231,7 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
@@ -6266,7 +6266,7 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
@@ -6406,7 +6406,7 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
@@ -6441,7 +6441,7 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G172" t="inlineStr">
@@ -6476,7 +6476,7 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G173" t="inlineStr">
@@ -6511,7 +6511,7 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G174" t="inlineStr">
@@ -6546,7 +6546,7 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G175" t="inlineStr">
@@ -6616,7 +6616,7 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G177" t="inlineStr">
@@ -6651,7 +6651,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
@@ -6686,7 +6686,7 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
@@ -6721,7 +6721,7 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G180" t="inlineStr">
@@ -6756,7 +6756,7 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G181" t="inlineStr">
@@ -6826,7 +6826,7 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G183" t="inlineStr">
@@ -6896,7 +6896,7 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
@@ -6931,7 +6931,7 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G186" t="inlineStr">
@@ -6966,7 +6966,7 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
@@ -7001,7 +7001,7 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
@@ -7176,7 +7176,7 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G193" t="inlineStr">
@@ -7211,7 +7211,7 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
@@ -7316,7 +7316,7 @@
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G197" t="inlineStr">
@@ -7456,7 +7456,7 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G201" t="inlineStr">
@@ -7491,7 +7491,7 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G202" t="inlineStr">
@@ -7526,7 +7526,7 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
@@ -7561,7 +7561,7 @@
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
@@ -7596,7 +7596,7 @@
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G205" t="inlineStr">
@@ -7636,7 +7636,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bo</t>
         </is>
       </c>
     </row>
@@ -7666,12 +7666,12 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -7706,7 +7706,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bo</t>
         </is>
       </c>
     </row>
@@ -7736,12 +7736,12 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -7771,7 +7771,7 @@
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G210" t="inlineStr">
@@ -7806,7 +7806,7 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G211" t="inlineStr">
@@ -7841,7 +7841,7 @@
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G212" t="inlineStr">
@@ -7911,7 +7911,7 @@
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
@@ -7946,7 +7946,7 @@
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
@@ -7981,7 +7981,7 @@
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
@@ -8051,7 +8051,7 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
@@ -8086,7 +8086,7 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
@@ -8191,7 +8191,7 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
@@ -8226,7 +8226,7 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
@@ -8296,7 +8296,7 @@
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
@@ -8331,7 +8331,7 @@
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
@@ -8401,7 +8401,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
@@ -8646,7 +8646,7 @@
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
@@ -8681,7 +8681,7 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
@@ -8716,7 +8716,7 @@
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
@@ -8751,7 +8751,7 @@
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G238" t="inlineStr">
@@ -8786,7 +8786,7 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
@@ -8856,7 +8856,7 @@
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G241" t="inlineStr">
@@ -8891,7 +8891,7 @@
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G242" t="inlineStr">
@@ -8926,7 +8926,7 @@
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G243" t="inlineStr">
@@ -8961,7 +8961,7 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
@@ -8996,7 +8996,7 @@
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G245" t="inlineStr">
@@ -9066,7 +9066,7 @@
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G247" t="inlineStr">
@@ -9171,7 +9171,7 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G250" t="inlineStr">
@@ -9241,7 +9241,7 @@
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G252" t="inlineStr">
@@ -9311,7 +9311,7 @@
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G254" t="inlineStr">
@@ -9346,7 +9346,7 @@
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G255" t="inlineStr">
@@ -9416,7 +9416,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G257" t="inlineStr">
@@ -9521,7 +9521,7 @@
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G260" t="inlineStr">
@@ -9556,7 +9556,7 @@
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G261" t="inlineStr">
@@ -9591,7 +9591,7 @@
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G262" t="inlineStr">
@@ -9801,7 +9801,7 @@
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
       <c r="G268" t="inlineStr">
@@ -9836,7 +9836,7 @@
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="G269" t="inlineStr">
@@ -9876,7 +9876,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -9906,12 +9906,12 @@
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -9946,7 +9946,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -9976,12 +9976,12 @@
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -10151,7 +10151,7 @@
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
@@ -10221,7 +10221,7 @@
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G280" t="inlineStr">
@@ -10256,7 +10256,7 @@
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
@@ -10326,7 +10326,7 @@
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
@@ -10361,7 +10361,7 @@
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G284" t="inlineStr">
@@ -10431,7 +10431,7 @@
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
@@ -10501,7 +10501,7 @@
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="G288" t="inlineStr">
@@ -10571,7 +10571,7 @@
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
@@ -10606,7 +10606,7 @@
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
@@ -10641,7 +10641,7 @@
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G292" t="inlineStr">
@@ -10711,7 +10711,7 @@
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="G294" t="inlineStr">
@@ -10746,7 +10746,7 @@
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
@@ -10781,7 +10781,7 @@
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
@@ -10816,7 +10816,7 @@
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
@@ -10886,7 +10886,7 @@
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G299" t="inlineStr">
@@ -10921,7 +10921,7 @@
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
@@ -10956,7 +10956,7 @@
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G301" t="inlineStr">
@@ -11026,7 +11026,7 @@
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
@@ -11061,7 +11061,7 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
@@ -11131,7 +11131,7 @@
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G306" t="inlineStr">
@@ -11201,7 +11201,7 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
@@ -11236,7 +11236,7 @@
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G309" t="inlineStr">
@@ -11306,7 +11306,7 @@
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G311" t="inlineStr">
@@ -11376,7 +11376,7 @@
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G313" t="inlineStr">
@@ -11446,7 +11446,7 @@
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G315" t="inlineStr">
@@ -11516,7 +11516,7 @@
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G317" t="inlineStr">
@@ -11551,7 +11551,7 @@
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G318" t="inlineStr">
@@ -11621,7 +11621,7 @@
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G320" t="inlineStr">
@@ -11656,7 +11656,7 @@
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G321" t="inlineStr">
@@ -11726,7 +11726,7 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G323" t="inlineStr">
@@ -11761,7 +11761,7 @@
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G324" t="inlineStr">
@@ -11831,7 +11831,7 @@
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G326" t="inlineStr">
@@ -11866,7 +11866,7 @@
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G327" t="inlineStr">
@@ -11901,7 +11901,7 @@
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G328" t="inlineStr">
@@ -11936,7 +11936,7 @@
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G329" t="inlineStr">
@@ -11971,7 +11971,7 @@
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G330" t="inlineStr">
@@ -12006,7 +12006,7 @@
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G331" t="inlineStr">
@@ -12041,7 +12041,7 @@
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G332" t="inlineStr">
@@ -12076,7 +12076,7 @@
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G333" t="inlineStr">
@@ -12111,7 +12111,7 @@
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G334" t="inlineStr">
@@ -12146,7 +12146,7 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G335" t="inlineStr">
@@ -12181,7 +12181,7 @@
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G336" t="inlineStr">
@@ -12216,7 +12216,7 @@
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G337" t="inlineStr">
@@ -12286,7 +12286,7 @@
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G339" t="inlineStr">
@@ -12321,7 +12321,7 @@
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G340" t="inlineStr">
@@ -12426,7 +12426,7 @@
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G343" t="inlineStr">
@@ -12496,7 +12496,7 @@
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G345" t="inlineStr">
@@ -12706,7 +12706,7 @@
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G351" t="inlineStr">
@@ -12741,7 +12741,7 @@
       </c>
       <c r="F352" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G352" t="inlineStr">
@@ -12846,7 +12846,7 @@
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G355" t="inlineStr">
@@ -12986,7 +12986,7 @@
       </c>
       <c r="F359" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G359" t="inlineStr">
@@ -13056,7 +13056,7 @@
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G361" t="inlineStr">
@@ -13091,7 +13091,7 @@
       </c>
       <c r="F362" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G362" t="inlineStr">
@@ -13126,7 +13126,7 @@
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G363" t="inlineStr">
@@ -13231,7 +13231,7 @@
       </c>
       <c r="F366" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G366" t="inlineStr">
@@ -13266,7 +13266,7 @@
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G367" t="inlineStr">
@@ -13301,7 +13301,7 @@
       </c>
       <c r="F368" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G368" t="inlineStr">
@@ -13336,7 +13336,7 @@
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G369" t="inlineStr">
@@ -13371,7 +13371,7 @@
       </c>
       <c r="F370" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G370" t="inlineStr">
@@ -13406,7 +13406,7 @@
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G371" t="inlineStr">
@@ -13441,7 +13441,7 @@
       </c>
       <c r="F372" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G372" t="inlineStr">
@@ -13511,7 +13511,7 @@
       </c>
       <c r="F374" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G374" t="inlineStr">
@@ -13581,7 +13581,7 @@
       </c>
       <c r="F376" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G376" t="inlineStr">
@@ -13651,7 +13651,7 @@
       </c>
       <c r="F378" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="G378" t="inlineStr">
@@ -13686,7 +13686,7 @@
       </c>
       <c r="F379" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G379" t="inlineStr">
@@ -13721,7 +13721,7 @@
       </c>
       <c r="F380" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G380" t="inlineStr">
@@ -13756,7 +13756,7 @@
       </c>
       <c r="F381" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G381" t="inlineStr">
@@ -13791,7 +13791,7 @@
       </c>
       <c r="F382" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G382" t="inlineStr">
@@ -13826,7 +13826,7 @@
       </c>
       <c r="F383" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G383" t="inlineStr">
@@ -13861,7 +13861,7 @@
       </c>
       <c r="F384" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G384" t="inlineStr">
@@ -13896,7 +13896,7 @@
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G385" t="inlineStr">
@@ -13931,7 +13931,7 @@
       </c>
       <c r="F386" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G386" t="inlineStr">
@@ -13966,7 +13966,7 @@
       </c>
       <c r="F387" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G387" t="inlineStr">
@@ -14001,7 +14001,7 @@
       </c>
       <c r="F388" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G388" t="inlineStr">
@@ -14036,7 +14036,7 @@
       </c>
       <c r="F389" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G389" t="inlineStr">
@@ -14071,7 +14071,7 @@
       </c>
       <c r="F390" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G390" t="inlineStr">
@@ -14106,7 +14106,7 @@
       </c>
       <c r="F391" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G391" t="inlineStr">
@@ -14141,7 +14141,7 @@
       </c>
       <c r="F392" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G392" t="inlineStr">
@@ -14176,7 +14176,7 @@
       </c>
       <c r="F393" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G393" t="inlineStr">
@@ -14211,7 +14211,7 @@
       </c>
       <c r="F394" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G394" t="inlineStr">
@@ -14246,7 +14246,7 @@
       </c>
       <c r="F395" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G395" t="inlineStr">
@@ -14281,7 +14281,7 @@
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G396" t="inlineStr">
@@ -14316,7 +14316,7 @@
       </c>
       <c r="F397" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G397" t="inlineStr">
@@ -14351,7 +14351,7 @@
       </c>
       <c r="F398" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G398" t="inlineStr">
@@ -14386,7 +14386,7 @@
       </c>
       <c r="F399" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G399" t="inlineStr">
@@ -14456,7 +14456,7 @@
       </c>
       <c r="F401" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G401" t="inlineStr">
@@ -14561,7 +14561,7 @@
       </c>
       <c r="F404" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G404" t="inlineStr">
@@ -14806,7 +14806,7 @@
       </c>
       <c r="F411" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G411" t="inlineStr">
@@ -14911,7 +14911,7 @@
       </c>
       <c r="F414" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G414" t="inlineStr">
@@ -14946,7 +14946,7 @@
       </c>
       <c r="F415" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G415" t="inlineStr">
@@ -15016,7 +15016,7 @@
       </c>
       <c r="F417" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G417" t="inlineStr">
@@ -15051,12 +15051,12 @@
       </c>
       <c r="F418" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G418" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -15086,12 +15086,12 @@
       </c>
       <c r="F419" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
       <c r="G419" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -15121,12 +15121,12 @@
       </c>
       <c r="F420" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>sa</t>
         </is>
       </c>
     </row>
@@ -15156,7 +15156,7 @@
       </c>
       <c r="F421" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G421" t="inlineStr">
@@ -15226,7 +15226,7 @@
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G423" t="inlineStr">
@@ -15261,7 +15261,7 @@
       </c>
       <c r="F424" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G424" t="inlineStr">
@@ -15296,7 +15296,7 @@
       </c>
       <c r="F425" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G425" t="inlineStr">
@@ -15331,7 +15331,7 @@
       </c>
       <c r="F426" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G426" t="inlineStr">
@@ -15366,7 +15366,7 @@
       </c>
       <c r="F427" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G427" t="inlineStr">
@@ -15436,7 +15436,7 @@
       </c>
       <c r="F429" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="G429" t="inlineStr">
@@ -15471,7 +15471,7 @@
       </c>
       <c r="F430" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G430" t="inlineStr">
@@ -15576,7 +15576,7 @@
       </c>
       <c r="F433" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G433" t="inlineStr">
@@ -15681,7 +15681,7 @@
       </c>
       <c r="F436" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G436" t="inlineStr">
@@ -15716,7 +15716,7 @@
       </c>
       <c r="F437" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G437" t="inlineStr">
@@ -15821,7 +15821,7 @@
       </c>
       <c r="F440" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G440" t="inlineStr">
@@ -15926,7 +15926,7 @@
       </c>
       <c r="F443" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G443" t="inlineStr">
@@ -15996,7 +15996,7 @@
       </c>
       <c r="F445" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
       <c r="G445" t="inlineStr">
@@ -16066,7 +16066,7 @@
       </c>
       <c r="F447" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G447" t="inlineStr">
@@ -16101,7 +16101,7 @@
       </c>
       <c r="F448" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G448" t="inlineStr">
@@ -16136,7 +16136,7 @@
       </c>
       <c r="F449" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G449" t="inlineStr">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="F459" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G459" t="inlineStr">
@@ -17256,7 +17256,7 @@
       </c>
       <c r="F481" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G481" t="inlineStr">
@@ -22961,7 +22961,7 @@
       </c>
       <c r="F644" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="G644" t="inlineStr">
@@ -23836,7 +23836,7 @@
       </c>
       <c r="F669" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G669" t="inlineStr">
@@ -24186,7 +24186,7 @@
       </c>
       <c r="F679" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G679" t="inlineStr">
@@ -25726,7 +25726,7 @@
       </c>
       <c r="F723" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G723" t="inlineStr">
@@ -25761,7 +25761,7 @@
       </c>
       <c r="F724" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G724" t="inlineStr">
@@ -25971,7 +25971,7 @@
       </c>
       <c r="F730" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G730" t="inlineStr">
@@ -26006,7 +26006,7 @@
       </c>
       <c r="F731" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G731" t="inlineStr">
@@ -26041,7 +26041,7 @@
       </c>
       <c r="F732" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G732" t="inlineStr">
@@ -26076,7 +26076,7 @@
       </c>
       <c r="F733" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G733" t="inlineStr">
@@ -26111,7 +26111,7 @@
       </c>
       <c r="F734" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G734" t="inlineStr">
@@ -26146,7 +26146,7 @@
       </c>
       <c r="F735" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G735" t="inlineStr">
@@ -26181,7 +26181,7 @@
       </c>
       <c r="F736" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G736" t="inlineStr">
@@ -26356,7 +26356,7 @@
       </c>
       <c r="F741" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G741" t="inlineStr">
@@ -26496,7 +26496,7 @@
       </c>
       <c r="F745" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G745" t="inlineStr">
@@ -26566,7 +26566,7 @@
       </c>
       <c r="F747" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G747" t="inlineStr">
@@ -26601,7 +26601,7 @@
       </c>
       <c r="F748" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G748" t="inlineStr">
@@ -26741,7 +26741,7 @@
       </c>
       <c r="F752" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="G752" t="inlineStr">
@@ -26776,7 +26776,7 @@
       </c>
       <c r="F753" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G753" t="inlineStr">
@@ -26846,7 +26846,7 @@
       </c>
       <c r="F755" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="G755" t="inlineStr">
@@ -27021,7 +27021,7 @@
       </c>
       <c r="F760" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
       <c r="G760" t="inlineStr">
@@ -27056,7 +27056,7 @@
       </c>
       <c r="F761" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="G761" t="inlineStr">
@@ -27126,7 +27126,7 @@
       </c>
       <c r="F763" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
       <c r="G763" t="inlineStr">
@@ -27161,7 +27161,7 @@
       </c>
       <c r="F764" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="G764" t="inlineStr">
@@ -27196,7 +27196,7 @@
       </c>
       <c r="F765" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G765" t="inlineStr">
@@ -27266,7 +27266,7 @@
       </c>
       <c r="F767" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G767" t="inlineStr">
@@ -27336,7 +27336,7 @@
       </c>
       <c r="F769" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G769" t="inlineStr">
@@ -27371,7 +27371,7 @@
       </c>
       <c r="F770" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G770" t="inlineStr">
@@ -27441,7 +27441,7 @@
       </c>
       <c r="F772" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G772" t="inlineStr">
@@ -27476,7 +27476,7 @@
       </c>
       <c r="F773" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G773" t="inlineStr">
@@ -27546,7 +27546,7 @@
       </c>
       <c r="F775" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G775" t="inlineStr">
@@ -27581,7 +27581,7 @@
       </c>
       <c r="F776" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G776" t="inlineStr">
@@ -27651,7 +27651,7 @@
       </c>
       <c r="F778" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G778" t="inlineStr">
@@ -27686,7 +27686,7 @@
       </c>
       <c r="F779" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G779" t="inlineStr">
@@ -27756,7 +27756,7 @@
       </c>
       <c r="F781" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G781" t="inlineStr">
@@ -27791,7 +27791,7 @@
       </c>
       <c r="F782" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G782" t="inlineStr">
@@ -27861,7 +27861,7 @@
       </c>
       <c r="F784" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G784" t="inlineStr">
@@ -27931,7 +27931,7 @@
       </c>
       <c r="F786" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G786" t="inlineStr">
@@ -27966,7 +27966,7 @@
       </c>
       <c r="F787" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G787" t="inlineStr">
@@ -28036,7 +28036,7 @@
       </c>
       <c r="F789" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G789" t="inlineStr">
@@ -28071,7 +28071,7 @@
       </c>
       <c r="F790" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G790" t="inlineStr">
@@ -28141,7 +28141,7 @@
       </c>
       <c r="F792" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G792" t="inlineStr">
@@ -28176,7 +28176,7 @@
       </c>
       <c r="F793" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G793" t="inlineStr">
@@ -28246,7 +28246,7 @@
       </c>
       <c r="F795" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G795" t="inlineStr">
@@ -28281,7 +28281,7 @@
       </c>
       <c r="F796" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G796" t="inlineStr">
@@ -28351,7 +28351,7 @@
       </c>
       <c r="F798" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G798" t="inlineStr">
@@ -28491,7 +28491,7 @@
       </c>
       <c r="F802" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G802" t="inlineStr">
@@ -28596,7 +28596,7 @@
       </c>
       <c r="F805" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G805" t="inlineStr">
@@ -28736,7 +28736,7 @@
       </c>
       <c r="F809" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G809" t="inlineStr">
@@ -28771,7 +28771,7 @@
       </c>
       <c r="F810" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G810" t="inlineStr">
@@ -28806,7 +28806,7 @@
       </c>
       <c r="F811" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G811" t="inlineStr">
@@ -28876,7 +28876,7 @@
       </c>
       <c r="F813" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G813" t="inlineStr">
@@ -28981,7 +28981,7 @@
       </c>
       <c r="F816" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G816" t="inlineStr">
@@ -29016,7 +29016,7 @@
       </c>
       <c r="F817" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G817" t="inlineStr">
@@ -29086,7 +29086,7 @@
       </c>
       <c r="F819" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G819" t="inlineStr">
@@ -29156,7 +29156,7 @@
       </c>
       <c r="F821" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G821" t="inlineStr">
@@ -29261,7 +29261,7 @@
       </c>
       <c r="F824" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G824" t="inlineStr">
@@ -29471,7 +29471,7 @@
       </c>
       <c r="F830" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G830" t="inlineStr">
@@ -29541,7 +29541,7 @@
       </c>
       <c r="F832" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G832" t="inlineStr">
@@ -29576,7 +29576,7 @@
       </c>
       <c r="F833" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G833" t="inlineStr">
@@ -29646,7 +29646,7 @@
       </c>
       <c r="F835" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G835" t="inlineStr">
@@ -29681,7 +29681,7 @@
       </c>
       <c r="F836" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G836" t="inlineStr">
@@ -29751,7 +29751,7 @@
       </c>
       <c r="F838" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G838" t="inlineStr">
@@ -29786,7 +29786,7 @@
       </c>
       <c r="F839" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G839" t="inlineStr">
@@ -29856,7 +29856,7 @@
       </c>
       <c r="F841" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G841" t="inlineStr">
@@ -29891,7 +29891,7 @@
       </c>
       <c r="F842" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G842" t="inlineStr">
@@ -29961,7 +29961,7 @@
       </c>
       <c r="F844" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G844" t="inlineStr">
@@ -29996,7 +29996,7 @@
       </c>
       <c r="F845" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G845" t="inlineStr">
@@ -30031,7 +30031,7 @@
       </c>
       <c r="F846" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G846" t="inlineStr">
@@ -30066,7 +30066,7 @@
       </c>
       <c r="F847" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G847" t="inlineStr">
@@ -30101,7 +30101,7 @@
       </c>
       <c r="F848" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G848" t="inlineStr">
@@ -30276,7 +30276,7 @@
       </c>
       <c r="F853" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G853" t="inlineStr">
@@ -30346,7 +30346,7 @@
       </c>
       <c r="F855" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G855" t="inlineStr">
@@ -30381,7 +30381,7 @@
       </c>
       <c r="F856" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G856" t="inlineStr">
@@ -30451,7 +30451,7 @@
       </c>
       <c r="F858" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G858" t="inlineStr">
@@ -30556,7 +30556,7 @@
       </c>
       <c r="F861" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G861" t="inlineStr">
@@ -30591,7 +30591,7 @@
       </c>
       <c r="F862" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G862" t="inlineStr">
@@ -30626,7 +30626,7 @@
       </c>
       <c r="F863" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G863" t="inlineStr">
@@ -30661,7 +30661,7 @@
       </c>
       <c r="F864" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G864" t="inlineStr">
@@ -30696,7 +30696,7 @@
       </c>
       <c r="F865" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G865" t="inlineStr">
@@ -30731,7 +30731,7 @@
       </c>
       <c r="F866" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G866" t="inlineStr">
@@ -30801,7 +30801,7 @@
       </c>
       <c r="F868" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G868" t="inlineStr">
@@ -30871,7 +30871,7 @@
       </c>
       <c r="F870" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G870" t="inlineStr">
@@ -30906,7 +30906,7 @@
       </c>
       <c r="F871" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G871" t="inlineStr">
@@ -30976,7 +30976,7 @@
       </c>
       <c r="F873" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G873" t="inlineStr">
@@ -31046,7 +31046,7 @@
       </c>
       <c r="F875" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G875" t="inlineStr">
@@ -31116,7 +31116,7 @@
       </c>
       <c r="F877" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G877" t="inlineStr">
@@ -31186,7 +31186,7 @@
       </c>
       <c r="F879" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G879" t="inlineStr">
@@ -31221,7 +31221,7 @@
       </c>
       <c r="F880" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G880" t="inlineStr">
@@ -31291,7 +31291,7 @@
       </c>
       <c r="F882" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G882" t="inlineStr">
@@ -31361,7 +31361,7 @@
       </c>
       <c r="F884" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G884" t="inlineStr">
@@ -31396,7 +31396,7 @@
       </c>
       <c r="F885" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G885" t="inlineStr">
@@ -31466,7 +31466,7 @@
       </c>
       <c r="F887" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G887" t="inlineStr">
@@ -31536,7 +31536,7 @@
       </c>
       <c r="F889" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G889" t="inlineStr">
@@ -31571,7 +31571,7 @@
       </c>
       <c r="F890" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G890" t="inlineStr">
@@ -31641,7 +31641,7 @@
       </c>
       <c r="F892" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G892" t="inlineStr">
@@ -31711,7 +31711,7 @@
       </c>
       <c r="F894" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G894" t="inlineStr">
@@ -31746,7 +31746,7 @@
       </c>
       <c r="F895" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G895" t="inlineStr">
@@ -31816,7 +31816,7 @@
       </c>
       <c r="F897" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G897" t="inlineStr">
@@ -31886,7 +31886,7 @@
       </c>
       <c r="F899" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G899" t="inlineStr">
@@ -31921,7 +31921,7 @@
       </c>
       <c r="F900" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G900" t="inlineStr">
@@ -31991,7 +31991,7 @@
       </c>
       <c r="F902" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G902" t="inlineStr">
@@ -32026,7 +32026,7 @@
       </c>
       <c r="F903" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G903" t="inlineStr">
@@ -32096,7 +32096,7 @@
       </c>
       <c r="F905" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G905" t="inlineStr">
@@ -32166,7 +32166,7 @@
       </c>
       <c r="F907" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="G907" t="inlineStr">
@@ -32201,7 +32201,7 @@
       </c>
       <c r="F908" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G908" t="inlineStr">
@@ -32271,7 +32271,7 @@
       </c>
       <c r="F910" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="G910" t="inlineStr">
@@ -32306,7 +32306,7 @@
       </c>
       <c r="F911" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G911" t="inlineStr">
@@ -32341,7 +32341,7 @@
       </c>
       <c r="F912" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G912" t="inlineStr">
@@ -32411,7 +32411,7 @@
       </c>
       <c r="F914" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G914" t="inlineStr">
@@ -32446,7 +32446,7 @@
       </c>
       <c r="F915" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G915" t="inlineStr">
@@ -32516,7 +32516,7 @@
       </c>
       <c r="F917" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G917" t="inlineStr">
@@ -32551,7 +32551,7 @@
       </c>
       <c r="F918" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G918" t="inlineStr">
@@ -32621,7 +32621,7 @@
       </c>
       <c r="F920" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G920" t="inlineStr">
@@ -32656,7 +32656,7 @@
       </c>
       <c r="F921" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G921" t="inlineStr">
@@ -32726,7 +32726,7 @@
       </c>
       <c r="F923" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G923" t="inlineStr">
@@ -32901,7 +32901,7 @@
       </c>
       <c r="F928" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G928" t="inlineStr">
@@ -32971,7 +32971,7 @@
       </c>
       <c r="F930" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G930" t="inlineStr">
@@ -33041,7 +33041,7 @@
       </c>
       <c r="F932" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G932" t="inlineStr">
@@ -33216,7 +33216,7 @@
       </c>
       <c r="F937" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G937" t="inlineStr">
@@ -33286,7 +33286,7 @@
       </c>
       <c r="F939" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G939" t="inlineStr">
@@ -33321,7 +33321,7 @@
       </c>
       <c r="F940" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G940" t="inlineStr">
@@ -33391,7 +33391,7 @@
       </c>
       <c r="F942" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G942" t="inlineStr">
@@ -33426,7 +33426,7 @@
       </c>
       <c r="F943" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G943" t="inlineStr">
@@ -33461,7 +33461,7 @@
       </c>
       <c r="F944" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G944" t="inlineStr">
@@ -33496,7 +33496,7 @@
       </c>
       <c r="F945" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G945" t="inlineStr">
@@ -33601,7 +33601,7 @@
       </c>
       <c r="F948" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G948" t="inlineStr">
@@ -33706,7 +33706,7 @@
       </c>
       <c r="F951" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G951" t="inlineStr">
@@ -33741,7 +33741,7 @@
       </c>
       <c r="F952" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G952" t="inlineStr">
@@ -33776,7 +33776,7 @@
       </c>
       <c r="F953" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G953" t="inlineStr">
@@ -33811,7 +33811,7 @@
       </c>
       <c r="F954" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G954" t="inlineStr">
@@ -33846,7 +33846,7 @@
       </c>
       <c r="F955" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G955" t="inlineStr">
@@ -33881,7 +33881,7 @@
       </c>
       <c r="F956" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G956" t="inlineStr">
@@ -33951,7 +33951,7 @@
       </c>
       <c r="F958" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G958" t="inlineStr">
@@ -33986,7 +33986,7 @@
       </c>
       <c r="F959" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G959" t="inlineStr">
@@ -34056,7 +34056,7 @@
       </c>
       <c r="F961" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G961" t="inlineStr">
@@ -34091,7 +34091,7 @@
       </c>
       <c r="F962" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G962" t="inlineStr">
@@ -34126,7 +34126,7 @@
       </c>
       <c r="F963" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G963" t="inlineStr">
@@ -34161,7 +34161,7 @@
       </c>
       <c r="F964" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G964" t="inlineStr">
@@ -34196,7 +34196,7 @@
       </c>
       <c r="F965" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G965" t="inlineStr">
@@ -34231,7 +34231,7 @@
       </c>
       <c r="F966" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G966" t="inlineStr">
@@ -34266,7 +34266,7 @@
       </c>
       <c r="F967" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G967" t="inlineStr">
@@ -34301,7 +34301,7 @@
       </c>
       <c r="F968" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G968" t="inlineStr">
@@ -34441,7 +34441,7 @@
       </c>
       <c r="F972" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G972" t="inlineStr">
@@ -34546,7 +34546,7 @@
       </c>
       <c r="F975" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G975" t="inlineStr">
@@ -34581,7 +34581,7 @@
       </c>
       <c r="F976" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G976" t="inlineStr">
@@ -34616,7 +34616,7 @@
       </c>
       <c r="F977" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G977" t="inlineStr">
@@ -34651,7 +34651,7 @@
       </c>
       <c r="F978" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G978" t="inlineStr">
@@ -35666,7 +35666,7 @@
       </c>
       <c r="F1007" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G1007" t="inlineStr">
@@ -35701,7 +35701,7 @@
       </c>
       <c r="F1008" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1008" t="inlineStr">
@@ -35736,7 +35736,7 @@
       </c>
       <c r="F1009" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G1009" t="inlineStr">
@@ -35771,7 +35771,7 @@
       </c>
       <c r="F1010" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1010" t="inlineStr">
@@ -35841,7 +35841,7 @@
       </c>
       <c r="F1012" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1012" t="inlineStr">
@@ -35911,7 +35911,7 @@
       </c>
       <c r="F1014" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1014" t="inlineStr">
@@ -35981,7 +35981,7 @@
       </c>
       <c r="F1016" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1016" t="inlineStr">
@@ -36401,7 +36401,7 @@
       </c>
       <c r="F1028" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G1028" t="inlineStr">
@@ -36436,7 +36436,7 @@
       </c>
       <c r="F1029" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1029" t="inlineStr">
@@ -36471,7 +36471,7 @@
       </c>
       <c r="F1030" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G1030" t="inlineStr">
@@ -36506,7 +36506,7 @@
       </c>
       <c r="F1031" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1031" t="inlineStr">
@@ -36541,7 +36541,7 @@
       </c>
       <c r="F1032" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G1032" t="inlineStr">
@@ -36576,7 +36576,7 @@
       </c>
       <c r="F1033" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1033" t="inlineStr">
@@ -36611,7 +36611,7 @@
       </c>
       <c r="F1034" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G1034" t="inlineStr">
@@ -36646,7 +36646,7 @@
       </c>
       <c r="F1035" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1035" t="inlineStr">
@@ -36681,7 +36681,7 @@
       </c>
       <c r="F1036" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G1036" t="inlineStr">
@@ -36786,7 +36786,7 @@
       </c>
       <c r="F1039" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G1039" t="inlineStr">
@@ -36891,7 +36891,7 @@
       </c>
       <c r="F1042" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G1042" t="inlineStr">
@@ -36996,7 +36996,7 @@
       </c>
       <c r="F1045" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="G1045" t="inlineStr">
@@ -37346,7 +37346,7 @@
       </c>
       <c r="F1055" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1055" t="inlineStr">
@@ -37381,7 +37381,7 @@
       </c>
       <c r="F1056" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1056" t="inlineStr">
@@ -37416,7 +37416,7 @@
       </c>
       <c r="F1057" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1057" t="inlineStr">
@@ -37451,7 +37451,7 @@
       </c>
       <c r="F1058" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1058" t="inlineStr">
@@ -37486,7 +37486,7 @@
       </c>
       <c r="F1059" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1059" t="inlineStr">
@@ -37521,7 +37521,7 @@
       </c>
       <c r="F1060" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1060" t="inlineStr">
@@ -37556,7 +37556,7 @@
       </c>
       <c r="F1061" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1061" t="inlineStr">
@@ -37591,7 +37591,7 @@
       </c>
       <c r="F1062" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1062" t="inlineStr">
@@ -37766,7 +37766,7 @@
       </c>
       <c r="F1067" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G1067" t="inlineStr">
@@ -37836,7 +37836,7 @@
       </c>
       <c r="F1069" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G1069" t="inlineStr">
@@ -37941,7 +37941,7 @@
       </c>
       <c r="F1072" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
       <c r="G1072" t="inlineStr">
@@ -38046,7 +38046,7 @@
       </c>
       <c r="F1075" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1075" t="inlineStr">
@@ -38116,7 +38116,7 @@
       </c>
       <c r="F1077" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1077" t="inlineStr">
@@ -38151,7 +38151,7 @@
       </c>
       <c r="F1078" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1078" t="inlineStr">
@@ -38221,7 +38221,7 @@
       </c>
       <c r="F1080" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1080" t="inlineStr">
@@ -38256,7 +38256,7 @@
       </c>
       <c r="F1081" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G1081" t="inlineStr">
@@ -38326,7 +38326,7 @@
       </c>
       <c r="F1083" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1083" t="inlineStr">
@@ -38431,7 +38431,7 @@
       </c>
       <c r="F1086" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1086" t="inlineStr">
@@ -38466,7 +38466,7 @@
       </c>
       <c r="F1087" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1087" t="inlineStr">
@@ -38536,7 +38536,7 @@
       </c>
       <c r="F1089" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1089" t="inlineStr">
@@ -38571,7 +38571,7 @@
       </c>
       <c r="F1090" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1090" t="inlineStr">
@@ -38641,7 +38641,7 @@
       </c>
       <c r="F1092" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1092" t="inlineStr">
@@ -38676,7 +38676,7 @@
       </c>
       <c r="F1093" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1093" t="inlineStr">
@@ -38746,7 +38746,7 @@
       </c>
       <c r="F1095" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1095" t="inlineStr">
@@ -38781,7 +38781,7 @@
       </c>
       <c r="F1096" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1096" t="inlineStr">
@@ -38851,7 +38851,7 @@
       </c>
       <c r="F1098" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1098" t="inlineStr">
@@ -38886,7 +38886,7 @@
       </c>
       <c r="F1099" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G1099" t="inlineStr">
@@ -38921,7 +38921,7 @@
       </c>
       <c r="F1100" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1100" t="inlineStr">
@@ -38956,7 +38956,7 @@
       </c>
       <c r="F1101" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1101" t="inlineStr">
@@ -38991,7 +38991,7 @@
       </c>
       <c r="F1102" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
       <c r="G1102" t="inlineStr">
@@ -39026,7 +39026,7 @@
       </c>
       <c r="F1103" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1103" t="inlineStr">
@@ -39096,7 +39096,7 @@
       </c>
       <c r="F1105" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
       <c r="G1105" t="inlineStr">
@@ -39166,7 +39166,7 @@
       </c>
       <c r="F1107" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
       <c r="G1107" t="inlineStr">
@@ -39586,7 +39586,7 @@
       </c>
       <c r="F1119" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G1119" t="inlineStr">
@@ -39621,7 +39621,7 @@
       </c>
       <c r="F1120" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1120" t="inlineStr">
@@ -39656,7 +39656,7 @@
       </c>
       <c r="F1121" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G1121" t="inlineStr">
@@ -39691,7 +39691,7 @@
       </c>
       <c r="F1122" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1122" t="inlineStr">
@@ -39726,7 +39726,7 @@
       </c>
       <c r="F1123" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G1123" t="inlineStr">
@@ -39761,7 +39761,7 @@
       </c>
       <c r="F1124" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1124" t="inlineStr">
@@ -39796,7 +39796,7 @@
       </c>
       <c r="F1125" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G1125" t="inlineStr">
@@ -39831,7 +39831,7 @@
       </c>
       <c r="F1126" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1126" t="inlineStr">
@@ -40006,7 +40006,7 @@
       </c>
       <c r="F1131" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G1131" t="inlineStr">
@@ -40076,7 +40076,7 @@
       </c>
       <c r="F1133" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="G1133" t="inlineStr">
@@ -40111,7 +40111,7 @@
       </c>
       <c r="F1134" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
       <c r="G1134" t="inlineStr">
@@ -40146,7 +40146,7 @@
       </c>
       <c r="F1135" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1135" t="inlineStr">
@@ -40181,7 +40181,7 @@
       </c>
       <c r="F1136" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1136" t="inlineStr">
@@ -40216,7 +40216,7 @@
       </c>
       <c r="F1137" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1137" t="inlineStr">
@@ -40251,7 +40251,7 @@
       </c>
       <c r="F1138" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1138" t="inlineStr">
@@ -40286,7 +40286,7 @@
       </c>
       <c r="F1139" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1139" t="inlineStr">
@@ -40321,7 +40321,7 @@
       </c>
       <c r="F1140" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1140" t="inlineStr">
@@ -40356,7 +40356,7 @@
       </c>
       <c r="F1141" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="G1141" t="inlineStr">
@@ -40391,7 +40391,7 @@
       </c>
       <c r="F1142" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1142" t="inlineStr">
@@ -40776,7 +40776,7 @@
       </c>
       <c r="F1153" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
       <c r="G1153" t="inlineStr">
@@ -40811,7 +40811,7 @@
       </c>
       <c r="F1154" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
       <c r="G1154" t="inlineStr">

</xml_diff>